<commit_message>
Restore status_pengiriman.xlsx dan tambahkan file data pengguna & kendaraan
</commit_message>
<xml_diff>
--- a/DASHBOARD_main/status_pengiriman.xlsx
+++ b/DASHBOARD_main/status_pengiriman.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,83 @@
           <t>Estimasi Terkirim</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Tanggal_Bayar</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>No_Resi</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Status_Pengiriman</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>4545454444444444</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>BG8888YY</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Siti Aminah</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Palembang</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>06-08-2025 14:37</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Pos Indonesia</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>RESI975880</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Diproses</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>08-08-2025 14:37</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>06-08-2025 14:37</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>RESI975880</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Diproses</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>